<commit_message>
Update frontend: convert images to WEBP format and update components
</commit_message>
<xml_diff>
--- a/bigclasses_backend/backend/media/enrollments/enrollments.xlsx
+++ b/bigclasses_backend/backend/media/enrollments/enrollments.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,10 +422,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="21" customWidth="1" min="1" max="1"/>
-    <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="2" max="2"/>
+    <col width="32" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -560,6 +560,60 @@
       <c r="E5" t="inlineStr">
         <is>
           <t>1233312131</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-05-21 15:29:45</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>LOKESWAR RAJU GUNDLAPALLI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>lokeshgundlapalli143@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>MLOps</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>08374705188</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-05-21 15:30:12</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>LOKESWAR RAJU GUNDLAPALLI</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>lokeshgundlapalli143@gmail.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Machine Learning</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>08374705188</t>
         </is>
       </c>
     </row>

</xml_diff>